<commit_message>
Adding non-rotating cipher, pretty color coding to show wires and real output values
</commit_message>
<xml_diff>
--- a/enigma workbook.xlsx
+++ b/enigma workbook.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/schultz/Desktop/git/enigma/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5A2761E8-7162-6744-BD03-7106A781CD17}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8FCCAA5F-5742-6249-8AE6-5C682C13D408}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1140" yWindow="820" windowWidth="28000" windowHeight="17440" activeTab="2" xr2:uid="{F6378511-5572-B14E-9156-0B5164924543}"/>
+    <workbookView xWindow="7400" yWindow="8260" windowWidth="28000" windowHeight="17440" activeTab="1" xr2:uid="{F6378511-5572-B14E-9156-0B5164924543}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -967,8 +967,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8B332738-11FB-2446-A1BF-E1B614445345}">
   <dimension ref="A1:I26"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="H1" sqref="H1:I26"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I27" sqref="I27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -976,7 +976,7 @@
     <row r="1" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A1">
         <f t="shared" ref="A1:A26" ca="1" si="0">RAND()</f>
-        <v>0.50019933661661575</v>
+        <v>0.25803513414605805</v>
       </c>
       <c r="B1">
         <v>4</v>
@@ -999,7 +999,7 @@
     <row r="2" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A2">
         <f t="shared" ca="1" si="0"/>
-        <v>0.99038038737180634</v>
+        <v>0.48471473984593816</v>
       </c>
       <c r="B2">
         <v>17</v>
@@ -1022,7 +1022,7 @@
     <row r="3" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A3">
         <f t="shared" ca="1" si="0"/>
-        <v>0.70880912716404831</v>
+        <v>0.69512068101540847</v>
       </c>
       <c r="B3">
         <v>19</v>
@@ -1045,7 +1045,7 @@
     <row r="4" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A4">
         <f t="shared" ca="1" si="0"/>
-        <v>0.61225999602735381</v>
+        <v>0.38843694239591098</v>
       </c>
       <c r="B4">
         <v>8</v>
@@ -1068,7 +1068,7 @@
     <row r="5" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A5">
         <f t="shared" ca="1" si="0"/>
-        <v>0.11689239564563147</v>
+        <v>0.63675700857511297</v>
       </c>
       <c r="B5">
         <v>14</v>
@@ -1091,7 +1091,7 @@
     <row r="6" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A6">
         <f t="shared" ca="1" si="0"/>
-        <v>0.66493293077272697</v>
+        <v>0.44440299389392668</v>
       </c>
       <c r="B6">
         <v>15</v>
@@ -1114,7 +1114,7 @@
     <row r="7" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A7">
         <f t="shared" ca="1" si="0"/>
-        <v>0.70946120938828261</v>
+        <v>0.61710621386646014</v>
       </c>
       <c r="B7">
         <v>2</v>
@@ -1137,7 +1137,7 @@
     <row r="8" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A8">
         <f t="shared" ca="1" si="0"/>
-        <v>0.13944795626492446</v>
+        <v>0.92768225331851473</v>
       </c>
       <c r="B8">
         <v>6</v>
@@ -1160,7 +1160,7 @@
     <row r="9" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A9">
         <f t="shared" ca="1" si="0"/>
-        <v>0.6721038062989223</v>
+        <v>0.47210066291048569</v>
       </c>
       <c r="B9">
         <v>0</v>
@@ -1183,7 +1183,7 @@
     <row r="10" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A10">
         <f t="shared" ca="1" si="0"/>
-        <v>0.80919651579601271</v>
+        <v>0.49154291343085854</v>
       </c>
       <c r="B10">
         <v>16</v>
@@ -1206,7 +1206,7 @@
     <row r="11" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A11">
         <f t="shared" ca="1" si="0"/>
-        <v>0.61738013185284313</v>
+        <v>0.7215976053960288</v>
       </c>
       <c r="B11">
         <v>10</v>
@@ -1229,7 +1229,7 @@
     <row r="12" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A12">
         <f t="shared" ca="1" si="0"/>
-        <v>0.78486225107068419</v>
+        <v>0.74805485457464449</v>
       </c>
       <c r="B12">
         <v>5</v>
@@ -1252,7 +1252,7 @@
     <row r="13" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A13">
         <f t="shared" ca="1" si="0"/>
-        <v>0.50281205682132568</v>
+        <v>0.71381381840671365</v>
       </c>
       <c r="B13">
         <v>20</v>
@@ -1275,7 +1275,7 @@
     <row r="14" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A14">
         <f t="shared" ca="1" si="0"/>
-        <v>0.97685708498450352</v>
+        <v>0.98247828701809414</v>
       </c>
       <c r="B14">
         <v>11</v>
@@ -1298,7 +1298,7 @@
     <row r="15" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A15">
         <f t="shared" ca="1" si="0"/>
-        <v>0.82240617951235795</v>
+        <v>0.76034008285764931</v>
       </c>
       <c r="B15">
         <v>9</v>
@@ -1321,7 +1321,7 @@
     <row r="16" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A16">
         <f t="shared" ca="1" si="0"/>
-        <v>0.9515342045584485</v>
+        <v>9.5222671236982026E-2</v>
       </c>
       <c r="B16">
         <v>7</v>
@@ -1344,7 +1344,7 @@
     <row r="17" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A17">
         <f t="shared" ca="1" si="0"/>
-        <v>0.99065747677054561</v>
+        <v>0.80079946626229659</v>
       </c>
       <c r="B17">
         <v>1</v>
@@ -1367,7 +1367,7 @@
     <row r="18" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A18">
         <f t="shared" ca="1" si="0"/>
-        <v>0.36295014984439389</v>
+        <v>0.83432230512477601</v>
       </c>
       <c r="B18">
         <v>3</v>
@@ -1390,7 +1390,7 @@
     <row r="19" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A19">
         <f t="shared" ca="1" si="0"/>
-        <v>0.39181547259142713</v>
+        <v>0.26470528844916785</v>
       </c>
       <c r="B19">
         <v>13</v>
@@ -1413,7 +1413,7 @@
     <row r="20" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A20">
         <f t="shared" ca="1" si="0"/>
-        <v>0.58606402709750016</v>
+        <v>0.17058571346690743</v>
       </c>
       <c r="B20">
         <v>25</v>
@@ -1436,7 +1436,7 @@
     <row r="21" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A21">
         <f t="shared" ca="1" si="0"/>
-        <v>0.67462900113855129</v>
+        <v>0.1283387855677941</v>
       </c>
       <c r="B21">
         <v>18</v>
@@ -1459,7 +1459,7 @@
     <row r="22" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A22">
         <f t="shared" ca="1" si="0"/>
-        <v>0.62520562546624281</v>
+        <v>0.10781144740727566</v>
       </c>
       <c r="B22">
         <v>22</v>
@@ -1482,7 +1482,7 @@
     <row r="23" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A23">
         <f t="shared" ca="1" si="0"/>
-        <v>0.18654917715179542</v>
+        <v>0.42900308211852833</v>
       </c>
       <c r="B23">
         <v>24</v>
@@ -1505,7 +1505,7 @@
     <row r="24" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A24">
         <f t="shared" ca="1" si="0"/>
-        <v>0.18625891279365248</v>
+        <v>0.4445598017280411</v>
       </c>
       <c r="B24">
         <v>23</v>
@@ -1528,7 +1528,7 @@
     <row r="25" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A25">
         <f t="shared" ca="1" si="0"/>
-        <v>0.68365097024383714</v>
+        <v>0.21495436072472995</v>
       </c>
       <c r="B25">
         <v>12</v>
@@ -1551,7 +1551,7 @@
     <row r="26" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A26">
         <f t="shared" ca="1" si="0"/>
-        <v>0.19908782116002577</v>
+        <v>0.32578833537191909</v>
       </c>
       <c r="B26">
         <v>21</v>
@@ -1584,7 +1584,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4246E425-7937-4C49-8B85-6B7A3D6A506D}">
   <dimension ref="A1:M26"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="M26" sqref="M26"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
adding configuration div to show the rotors and reflector state so they can eventually be changed
</commit_message>
<xml_diff>
--- a/enigma workbook.xlsx
+++ b/enigma workbook.xlsx
@@ -8,14 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/schultz/Desktop/git/enigma/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8FCCAA5F-5742-6249-8AE6-5C682C13D408}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1A298D46-8583-F04C-8958-B4BEE85C7421}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="7400" yWindow="8260" windowWidth="28000" windowHeight="17440" activeTab="1" xr2:uid="{F6378511-5572-B14E-9156-0B5164924543}"/>
+    <workbookView xWindow="11800" yWindow="2480" windowWidth="29120" windowHeight="20460" activeTab="3" xr2:uid="{F6378511-5572-B14E-9156-0B5164924543}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
+    <sheet name="reflector" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -38,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="80" uniqueCount="28">
   <si>
     <t>x</t>
   </si>
@@ -967,7 +968,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8B332738-11FB-2446-A1BF-E1B614445345}">
   <dimension ref="A1:I26"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="I27" sqref="I27"/>
     </sheetView>
   </sheetViews>
@@ -976,7 +977,7 @@
     <row r="1" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A1">
         <f t="shared" ref="A1:A26" ca="1" si="0">RAND()</f>
-        <v>0.25803513414605805</v>
+        <v>0.75207709460774941</v>
       </c>
       <c r="B1">
         <v>4</v>
@@ -999,7 +1000,7 @@
     <row r="2" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A2">
         <f t="shared" ca="1" si="0"/>
-        <v>0.48471473984593816</v>
+        <v>6.219636650086624E-4</v>
       </c>
       <c r="B2">
         <v>17</v>
@@ -1022,7 +1023,7 @@
     <row r="3" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A3">
         <f t="shared" ca="1" si="0"/>
-        <v>0.69512068101540847</v>
+        <v>6.4139827508703284E-2</v>
       </c>
       <c r="B3">
         <v>19</v>
@@ -1045,7 +1046,7 @@
     <row r="4" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A4">
         <f t="shared" ca="1" si="0"/>
-        <v>0.38843694239591098</v>
+        <v>0.38079033194203038</v>
       </c>
       <c r="B4">
         <v>8</v>
@@ -1068,7 +1069,7 @@
     <row r="5" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A5">
         <f t="shared" ca="1" si="0"/>
-        <v>0.63675700857511297</v>
+        <v>0.13122345521822243</v>
       </c>
       <c r="B5">
         <v>14</v>
@@ -1091,7 +1092,7 @@
     <row r="6" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A6">
         <f t="shared" ca="1" si="0"/>
-        <v>0.44440299389392668</v>
+        <v>0.89917811490820743</v>
       </c>
       <c r="B6">
         <v>15</v>
@@ -1114,7 +1115,7 @@
     <row r="7" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A7">
         <f t="shared" ca="1" si="0"/>
-        <v>0.61710621386646014</v>
+        <v>2.8756932923045486E-2</v>
       </c>
       <c r="B7">
         <v>2</v>
@@ -1137,7 +1138,7 @@
     <row r="8" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A8">
         <f t="shared" ca="1" si="0"/>
-        <v>0.92768225331851473</v>
+        <v>0.67450700285100662</v>
       </c>
       <c r="B8">
         <v>6</v>
@@ -1160,7 +1161,7 @@
     <row r="9" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A9">
         <f t="shared" ca="1" si="0"/>
-        <v>0.47210066291048569</v>
+        <v>0.20279520710362575</v>
       </c>
       <c r="B9">
         <v>0</v>
@@ -1183,7 +1184,7 @@
     <row r="10" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A10">
         <f t="shared" ca="1" si="0"/>
-        <v>0.49154291343085854</v>
+        <v>0.84646145808572104</v>
       </c>
       <c r="B10">
         <v>16</v>
@@ -1206,7 +1207,7 @@
     <row r="11" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A11">
         <f t="shared" ca="1" si="0"/>
-        <v>0.7215976053960288</v>
+        <v>8.685729820073762E-4</v>
       </c>
       <c r="B11">
         <v>10</v>
@@ -1229,7 +1230,7 @@
     <row r="12" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A12">
         <f t="shared" ca="1" si="0"/>
-        <v>0.74805485457464449</v>
+        <v>0.37840836989443338</v>
       </c>
       <c r="B12">
         <v>5</v>
@@ -1252,7 +1253,7 @@
     <row r="13" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A13">
         <f t="shared" ca="1" si="0"/>
-        <v>0.71381381840671365</v>
+        <v>0.34782229678240129</v>
       </c>
       <c r="B13">
         <v>20</v>
@@ -1275,7 +1276,7 @@
     <row r="14" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A14">
         <f t="shared" ca="1" si="0"/>
-        <v>0.98247828701809414</v>
+        <v>0.66953331123100179</v>
       </c>
       <c r="B14">
         <v>11</v>
@@ -1298,7 +1299,7 @@
     <row r="15" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A15">
         <f t="shared" ca="1" si="0"/>
-        <v>0.76034008285764931</v>
+        <v>0.52899885092668009</v>
       </c>
       <c r="B15">
         <v>9</v>
@@ -1321,7 +1322,7 @@
     <row r="16" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A16">
         <f t="shared" ca="1" si="0"/>
-        <v>9.5222671236982026E-2</v>
+        <v>0.21339964919833332</v>
       </c>
       <c r="B16">
         <v>7</v>
@@ -1344,7 +1345,7 @@
     <row r="17" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A17">
         <f t="shared" ca="1" si="0"/>
-        <v>0.80079946626229659</v>
+        <v>0.81990791718233202</v>
       </c>
       <c r="B17">
         <v>1</v>
@@ -1367,7 +1368,7 @@
     <row r="18" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A18">
         <f t="shared" ca="1" si="0"/>
-        <v>0.83432230512477601</v>
+        <v>0.33781554548371329</v>
       </c>
       <c r="B18">
         <v>3</v>
@@ -1390,7 +1391,7 @@
     <row r="19" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A19">
         <f t="shared" ca="1" si="0"/>
-        <v>0.26470528844916785</v>
+        <v>0.44068339234999099</v>
       </c>
       <c r="B19">
         <v>13</v>
@@ -1413,7 +1414,7 @@
     <row r="20" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A20">
         <f t="shared" ca="1" si="0"/>
-        <v>0.17058571346690743</v>
+        <v>0.94490872760996403</v>
       </c>
       <c r="B20">
         <v>25</v>
@@ -1436,7 +1437,7 @@
     <row r="21" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A21">
         <f t="shared" ca="1" si="0"/>
-        <v>0.1283387855677941</v>
+        <v>0.95409448723522383</v>
       </c>
       <c r="B21">
         <v>18</v>
@@ -1459,7 +1460,7 @@
     <row r="22" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A22">
         <f t="shared" ca="1" si="0"/>
-        <v>0.10781144740727566</v>
+        <v>0.57806673942343434</v>
       </c>
       <c r="B22">
         <v>22</v>
@@ -1482,7 +1483,7 @@
     <row r="23" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A23">
         <f t="shared" ca="1" si="0"/>
-        <v>0.42900308211852833</v>
+        <v>0.62697713959264001</v>
       </c>
       <c r="B23">
         <v>24</v>
@@ -1505,7 +1506,7 @@
     <row r="24" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A24">
         <f t="shared" ca="1" si="0"/>
-        <v>0.4445598017280411</v>
+        <v>0.87516349721423559</v>
       </c>
       <c r="B24">
         <v>23</v>
@@ -1528,7 +1529,7 @@
     <row r="25" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A25">
         <f t="shared" ca="1" si="0"/>
-        <v>0.21495436072472995</v>
+        <v>0.52110044810027767</v>
       </c>
       <c r="B25">
         <v>12</v>
@@ -1551,7 +1552,7 @@
     <row r="26" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A26">
         <f t="shared" ca="1" si="0"/>
-        <v>0.32578833537191909</v>
+        <v>0.83776297197700045</v>
       </c>
       <c r="B26">
         <v>21</v>
@@ -1585,7 +1586,7 @@
   <dimension ref="A1:M26"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="M26" sqref="M26"/>
+      <selection activeCell="I1" sqref="I1:I26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2217,4 +2218,435 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E83D9991-DF80-9143-8DE9-165CA3F83807}">
+  <dimension ref="B1:E26"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D2" sqref="D2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C1">
+        <v>0</v>
+      </c>
+      <c r="D1">
+        <v>1</v>
+      </c>
+      <c r="E1">
+        <f>D1</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B2" t="s">
+        <v>25</v>
+      </c>
+      <c r="C2">
+        <v>1</v>
+      </c>
+      <c r="D2">
+        <f>IF(ISODD(C2),C1,C3)</f>
+        <v>0</v>
+      </c>
+      <c r="E2" t="str">
+        <f>E1&amp;", "&amp;D2</f>
+        <v>1, 0</v>
+      </c>
+    </row>
+    <row r="3" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B3" t="s">
+        <v>23</v>
+      </c>
+      <c r="C3">
+        <v>2</v>
+      </c>
+      <c r="D3">
+        <f t="shared" ref="D3:D26" si="0">IF(ISODD(C3),C2,C4)</f>
+        <v>3</v>
+      </c>
+      <c r="E3" t="str">
+        <f>E2&amp;", "&amp;D3</f>
+        <v>1, 0, 3</v>
+      </c>
+    </row>
+    <row r="4" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B4" t="s">
+        <v>14</v>
+      </c>
+      <c r="C4">
+        <v>3</v>
+      </c>
+      <c r="D4">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+      <c r="E4" t="str">
+        <f t="shared" ref="E4:E26" si="1">E3&amp;", "&amp;D4</f>
+        <v>1, 0, 3, 2</v>
+      </c>
+    </row>
+    <row r="5" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B5" t="s">
+        <v>4</v>
+      </c>
+      <c r="C5">
+        <v>4</v>
+      </c>
+      <c r="D5">
+        <f t="shared" si="0"/>
+        <v>5</v>
+      </c>
+      <c r="E5" t="str">
+        <f t="shared" si="1"/>
+        <v>1, 0, 3, 2, 5</v>
+      </c>
+    </row>
+    <row r="6" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B6" t="s">
+        <v>15</v>
+      </c>
+      <c r="C6">
+        <v>5</v>
+      </c>
+      <c r="D6">
+        <f t="shared" si="0"/>
+        <v>4</v>
+      </c>
+      <c r="E6" t="str">
+        <f t="shared" si="1"/>
+        <v>1, 0, 3, 2, 5, 4</v>
+      </c>
+    </row>
+    <row r="7" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B7" t="s">
+        <v>16</v>
+      </c>
+      <c r="C7">
+        <v>6</v>
+      </c>
+      <c r="D7">
+        <f t="shared" si="0"/>
+        <v>7</v>
+      </c>
+      <c r="E7" t="str">
+        <f t="shared" si="1"/>
+        <v>1, 0, 3, 2, 5, 4, 7</v>
+      </c>
+    </row>
+    <row r="8" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B8" t="s">
+        <v>17</v>
+      </c>
+      <c r="C8">
+        <v>7</v>
+      </c>
+      <c r="D8">
+        <f t="shared" si="0"/>
+        <v>6</v>
+      </c>
+      <c r="E8" t="str">
+        <f t="shared" si="1"/>
+        <v>1, 0, 3, 2, 5, 4, 7, 6</v>
+      </c>
+    </row>
+    <row r="9" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B9" t="s">
+        <v>9</v>
+      </c>
+      <c r="C9">
+        <v>8</v>
+      </c>
+      <c r="D9">
+        <f t="shared" si="0"/>
+        <v>9</v>
+      </c>
+      <c r="E9" t="str">
+        <f t="shared" si="1"/>
+        <v>1, 0, 3, 2, 5, 4, 7, 6, 9</v>
+      </c>
+    </row>
+    <row r="10" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B10" t="s">
+        <v>18</v>
+      </c>
+      <c r="C10">
+        <v>9</v>
+      </c>
+      <c r="D10">
+        <f t="shared" si="0"/>
+        <v>8</v>
+      </c>
+      <c r="E10" t="str">
+        <f t="shared" si="1"/>
+        <v>1, 0, 3, 2, 5, 4, 7, 6, 9, 8</v>
+      </c>
+    </row>
+    <row r="11" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B11" t="s">
+        <v>19</v>
+      </c>
+      <c r="C11">
+        <v>10</v>
+      </c>
+      <c r="D11">
+        <f t="shared" si="0"/>
+        <v>11</v>
+      </c>
+      <c r="E11" t="str">
+        <f t="shared" si="1"/>
+        <v>1, 0, 3, 2, 5, 4, 7, 6, 9, 8, 11</v>
+      </c>
+    </row>
+    <row r="12" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B12" t="s">
+        <v>20</v>
+      </c>
+      <c r="C12">
+        <v>11</v>
+      </c>
+      <c r="D12">
+        <f t="shared" si="0"/>
+        <v>10</v>
+      </c>
+      <c r="E12" t="str">
+        <f t="shared" si="1"/>
+        <v>1, 0, 3, 2, 5, 4, 7, 6, 9, 8, 11, 10</v>
+      </c>
+    </row>
+    <row r="13" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B13" t="s">
+        <v>27</v>
+      </c>
+      <c r="C13">
+        <v>12</v>
+      </c>
+      <c r="D13">
+        <f t="shared" si="0"/>
+        <v>13</v>
+      </c>
+      <c r="E13" t="str">
+        <f t="shared" si="1"/>
+        <v>1, 0, 3, 2, 5, 4, 7, 6, 9, 8, 11, 10, 13</v>
+      </c>
+    </row>
+    <row r="14" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B14" t="s">
+        <v>26</v>
+      </c>
+      <c r="C14">
+        <v>13</v>
+      </c>
+      <c r="D14">
+        <f t="shared" si="0"/>
+        <v>12</v>
+      </c>
+      <c r="E14" t="str">
+        <f t="shared" si="1"/>
+        <v>1, 0, 3, 2, 5, 4, 7, 6, 9, 8, 11, 10, 13, 12</v>
+      </c>
+    </row>
+    <row r="15" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B15" t="s">
+        <v>10</v>
+      </c>
+      <c r="C15">
+        <v>14</v>
+      </c>
+      <c r="D15">
+        <f t="shared" si="0"/>
+        <v>15</v>
+      </c>
+      <c r="E15" t="str">
+        <f t="shared" si="1"/>
+        <v>1, 0, 3, 2, 5, 4, 7, 6, 9, 8, 11, 10, 13, 12, 15</v>
+      </c>
+    </row>
+    <row r="16" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B16" t="s">
+        <v>11</v>
+      </c>
+      <c r="C16">
+        <v>15</v>
+      </c>
+      <c r="D16">
+        <f t="shared" si="0"/>
+        <v>14</v>
+      </c>
+      <c r="E16" t="str">
+        <f t="shared" si="1"/>
+        <v>1, 0, 3, 2, 5, 4, 7, 6, 9, 8, 11, 10, 13, 12, 15, 14</v>
+      </c>
+    </row>
+    <row r="17" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B17" t="s">
+        <v>2</v>
+      </c>
+      <c r="C17">
+        <v>16</v>
+      </c>
+      <c r="D17">
+        <f t="shared" si="0"/>
+        <v>17</v>
+      </c>
+      <c r="E17" t="str">
+        <f t="shared" si="1"/>
+        <v>1, 0, 3, 2, 5, 4, 7, 6, 9, 8, 11, 10, 13, 12, 15, 14, 17</v>
+      </c>
+    </row>
+    <row r="18" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B18" t="s">
+        <v>5</v>
+      </c>
+      <c r="C18">
+        <v>17</v>
+      </c>
+      <c r="D18">
+        <f t="shared" si="0"/>
+        <v>16</v>
+      </c>
+      <c r="E18" t="str">
+        <f t="shared" si="1"/>
+        <v>1, 0, 3, 2, 5, 4, 7, 6, 9, 8, 11, 10, 13, 12, 15, 14, 17, 16</v>
+      </c>
+    </row>
+    <row r="19" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B19" t="s">
+        <v>13</v>
+      </c>
+      <c r="C19">
+        <v>18</v>
+      </c>
+      <c r="D19">
+        <f t="shared" si="0"/>
+        <v>19</v>
+      </c>
+      <c r="E19" t="str">
+        <f t="shared" si="1"/>
+        <v>1, 0, 3, 2, 5, 4, 7, 6, 9, 8, 11, 10, 13, 12, 15, 14, 17, 16, 19</v>
+      </c>
+    </row>
+    <row r="20" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B20" t="s">
+        <v>6</v>
+      </c>
+      <c r="C20">
+        <v>19</v>
+      </c>
+      <c r="D20">
+        <f t="shared" si="0"/>
+        <v>18</v>
+      </c>
+      <c r="E20" t="str">
+        <f t="shared" si="1"/>
+        <v>1, 0, 3, 2, 5, 4, 7, 6, 9, 8, 11, 10, 13, 12, 15, 14, 17, 16, 19, 18</v>
+      </c>
+    </row>
+    <row r="21" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B21" t="s">
+        <v>8</v>
+      </c>
+      <c r="C21">
+        <v>20</v>
+      </c>
+      <c r="D21">
+        <f t="shared" si="0"/>
+        <v>21</v>
+      </c>
+      <c r="E21" t="str">
+        <f t="shared" si="1"/>
+        <v>1, 0, 3, 2, 5, 4, 7, 6, 9, 8, 11, 10, 13, 12, 15, 14, 17, 16, 19, 18, 21</v>
+      </c>
+    </row>
+    <row r="22" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B22" t="s">
+        <v>24</v>
+      </c>
+      <c r="C22">
+        <v>21</v>
+      </c>
+      <c r="D22">
+        <f t="shared" si="0"/>
+        <v>20</v>
+      </c>
+      <c r="E22" t="str">
+        <f t="shared" si="1"/>
+        <v>1, 0, 3, 2, 5, 4, 7, 6, 9, 8, 11, 10, 13, 12, 15, 14, 17, 16, 19, 18, 21, 20</v>
+      </c>
+    </row>
+    <row r="23" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B23" t="s">
+        <v>3</v>
+      </c>
+      <c r="C23">
+        <v>22</v>
+      </c>
+      <c r="D23">
+        <f t="shared" si="0"/>
+        <v>23</v>
+      </c>
+      <c r="E23" t="str">
+        <f t="shared" si="1"/>
+        <v>1, 0, 3, 2, 5, 4, 7, 6, 9, 8, 11, 10, 13, 12, 15, 14, 17, 16, 19, 18, 21, 20, 23</v>
+      </c>
+    </row>
+    <row r="24" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B24" t="s">
+        <v>22</v>
+      </c>
+      <c r="C24">
+        <v>23</v>
+      </c>
+      <c r="D24">
+        <f t="shared" si="0"/>
+        <v>22</v>
+      </c>
+      <c r="E24" t="str">
+        <f t="shared" si="1"/>
+        <v>1, 0, 3, 2, 5, 4, 7, 6, 9, 8, 11, 10, 13, 12, 15, 14, 17, 16, 19, 18, 21, 20, 23, 22</v>
+      </c>
+    </row>
+    <row r="25" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B25" t="s">
+        <v>7</v>
+      </c>
+      <c r="C25">
+        <v>24</v>
+      </c>
+      <c r="D25">
+        <f t="shared" si="0"/>
+        <v>25</v>
+      </c>
+      <c r="E25" t="str">
+        <f t="shared" si="1"/>
+        <v>1, 0, 3, 2, 5, 4, 7, 6, 9, 8, 11, 10, 13, 12, 15, 14, 17, 16, 19, 18, 21, 20, 23, 22, 25</v>
+      </c>
+    </row>
+    <row r="26" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B26" t="s">
+        <v>21</v>
+      </c>
+      <c r="C26">
+        <v>25</v>
+      </c>
+      <c r="D26">
+        <f t="shared" si="0"/>
+        <v>24</v>
+      </c>
+      <c r="E26" t="str">
+        <f t="shared" si="1"/>
+        <v>1, 0, 3, 2, 5, 4, 7, 6, 9, 8, 11, 10, 13, 12, 15, 14, 17, 16, 19, 18, 21, 20, 23, 22, 25, 24</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
+</worksheet>
 </file>
</xml_diff>